<commit_message>
Buổi 4: React Base
</commit_message>
<xml_diff>
--- a/diem_danh_giay_06_03_23_07_39_59.xlsx
+++ b/diem_danh_giay_06_03_23_07_39_59.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowHeight="18800"/>
+    <workbookView windowHeight="16400"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,6 @@
   </si>
   <si>
     <t>Email</t>
-  </si>
-  <si>
-    <t>Điểm danh</t>
   </si>
   <si>
     <t>PH18767</t>
@@ -135,6 +132,9 @@
   </si>
   <si>
     <t>truongvhph24614@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
   <si>
     <t>PH24621</t>
@@ -422,13 +422,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="dd\-mmm"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -457,40 +458,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -504,37 +474,30 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -546,37 +509,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -592,6 +524,73 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -599,9 +598,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -613,12 +620,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -634,7 +635,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -646,7 +689,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -658,73 +773,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -736,67 +785,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -834,11 +841,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -858,26 +880,37 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -896,181 +929,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1094,9 +1101,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1485,8 +1494,8 @@
   <sheetPr/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1625,10 +1634,12 @@
       <c r="D5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>5</v>
+      <c r="E5" s="11">
+        <v>44991</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="12">
+        <v>44995</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1655,18 +1666,20 @@
         <v>1</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>9</v>
+      <c r="F6" s="1" t="s">
+        <v>8</v>
       </c>
-      <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1693,18 +1706,20 @@
         <v>2</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>12</v>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>9</v>
+      <c r="F7" s="1" t="s">
+        <v>8</v>
       </c>
-      <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -1731,18 +1746,20 @@
         <v>3</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>15</v>
+      <c r="E8" s="1" t="s">
+        <v>8</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>9</v>
+      <c r="F8" s="1" t="s">
+        <v>8</v>
       </c>
-      <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1769,18 +1786,20 @@
         <v>4</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>18</v>
+      <c r="E9" s="1" t="s">
+        <v>8</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>9</v>
+      <c r="F9" s="1" t="s">
+        <v>8</v>
       </c>
-      <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -1807,18 +1826,20 @@
         <v>5</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>21</v>
+      <c r="E10" s="1" t="s">
+        <v>8</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>9</v>
+      <c r="F10" s="1" t="s">
+        <v>8</v>
       </c>
-      <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -1845,18 +1866,20 @@
         <v>6</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>24</v>
+      <c r="E11" s="1" t="s">
+        <v>8</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>9</v>
+      <c r="F11" s="1" t="s">
+        <v>8</v>
       </c>
-      <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1883,18 +1906,20 @@
         <v>7</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>27</v>
+      <c r="E12" s="1" t="s">
+        <v>8</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>9</v>
+      <c r="F12" s="1" t="s">
+        <v>8</v>
       </c>
-      <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1921,18 +1946,20 @@
         <v>8</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="D13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>30</v>
+      <c r="E13" s="1" t="s">
+        <v>8</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>9</v>
+      <c r="F13" s="1" t="s">
+        <v>8</v>
       </c>
-      <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1959,18 +1986,20 @@
         <v>9</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="D14" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>33</v>
+      <c r="E14" s="1" t="s">
+        <v>8</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>9</v>
+      <c r="F14" s="1" t="s">
+        <v>8</v>
       </c>
-      <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1997,18 +2026,20 @@
         <v>10</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="D15" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>36</v>
+      <c r="E15" s="1" t="s">
+        <v>8</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>9</v>
+      <c r="F15" s="1" t="s">
+        <v>8</v>
       </c>
-      <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -2035,16 +2066,20 @@
         <v>11</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="D16" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="E16" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -2080,9 +2115,11 @@
         <v>42</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
-      <c r="F17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -2118,9 +2155,11 @@
         <v>45</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
-      <c r="F18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -2156,9 +2195,11 @@
         <v>48</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="F19" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -2194,9 +2235,11 @@
         <v>51</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
-      <c r="F20" s="1"/>
+      <c r="F20" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -2231,8 +2274,12 @@
       <c r="D21" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="E21" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>39</v>
+      </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -2268,9 +2315,11 @@
         <v>57</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
-      <c r="F22" s="1"/>
+      <c r="F22" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -2305,8 +2354,12 @@
       <c r="D23" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="E23" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -2342,9 +2395,11 @@
         <v>63</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
-      <c r="F24" s="1"/>
+      <c r="F24" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -2380,9 +2435,11 @@
         <v>66</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
-      <c r="F25" s="1"/>
+      <c r="F25" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -2418,9 +2475,11 @@
         <v>69</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
-      <c r="F26" s="1"/>
+      <c r="F26" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -2456,9 +2515,11 @@
         <v>72</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
-      <c r="F27" s="1"/>
+      <c r="F27" s="13" t="s">
+        <v>39</v>
+      </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -2494,9 +2555,11 @@
         <v>75</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
-      <c r="F28" s="1"/>
+      <c r="F28" s="13" t="s">
+        <v>39</v>
+      </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -2532,9 +2595,11 @@
         <v>78</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
-      <c r="F29" s="1"/>
+      <c r="F29" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -2569,8 +2634,12 @@
       <c r="D30" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
+      <c r="E30" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -2605,8 +2674,12 @@
       <c r="D31" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
+      <c r="E31" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -2642,9 +2715,11 @@
         <v>87</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
-      <c r="F32" s="1"/>
+      <c r="F32" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -2680,9 +2755,11 @@
         <v>90</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
-      <c r="F33" s="1"/>
+      <c r="F33" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -2718,9 +2795,11 @@
         <v>93</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
-      <c r="F34" s="1"/>
+      <c r="F34" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -2756,9 +2835,11 @@
         <v>96</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
-      <c r="F35" s="1"/>
+      <c r="F35" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -2794,9 +2875,11 @@
         <v>99</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
-      <c r="F36" s="1"/>
+      <c r="F36" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
@@ -2831,8 +2914,12 @@
       <c r="D37" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
+      <c r="E37" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
@@ -2868,9 +2955,11 @@
         <v>105</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
-      <c r="F38" s="1"/>
+      <c r="F38" s="13" t="s">
+        <v>39</v>
+      </c>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
@@ -2906,9 +2995,11 @@
         <v>108</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
-      <c r="F39" s="1"/>
+      <c r="F39" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
@@ -2944,9 +3035,11 @@
         <v>111</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
-      <c r="F40" s="1"/>
+      <c r="F40" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
@@ -2981,8 +3074,12 @@
       <c r="D41" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
+      <c r="E41" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>39</v>
+      </c>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
@@ -3018,9 +3115,11 @@
         <v>117</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
-      <c r="F42" s="1"/>
+      <c r="F42" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
@@ -3056,9 +3155,11 @@
         <v>120</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
-      <c r="F43" s="1"/>
+      <c r="F43" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
@@ -3093,8 +3194,12 @@
       <c r="D44" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
+      <c r="E44" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>

</xml_diff>

<commit_message>
Buổi 5: React - router
</commit_message>
<xml_diff>
--- a/diem_danh_giay_06_03_23_07_39_59.xlsx
+++ b/diem_danh_giay_06_03_23_07_39_59.xlsx
@@ -423,11 +423,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="dd\-mmm"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -463,87 +463,10 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -556,7 +479,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -571,7 +494,46 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -579,20 +541,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -608,7 +556,59 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -623,7 +623,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -635,13 +647,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -653,79 +755,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -737,43 +767,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -791,19 +785,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -832,11 +832,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -860,7 +866,18 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -880,6 +897,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -894,186 +929,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1494,8 +1494,8 @@
   <sheetPr/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1640,7 +1640,9 @@
       <c r="F5" s="12">
         <v>44995</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="G5" s="12">
+        <v>45000</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -1680,7 +1682,9 @@
       <c r="F6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -1720,7 +1724,9 @@
       <c r="F7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -1760,7 +1766,9 @@
       <c r="F8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -1800,7 +1808,9 @@
       <c r="F9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1840,7 +1850,9 @@
       <c r="F10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -1880,7 +1892,9 @@
       <c r="F11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="1"/>
+      <c r="G11" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1920,7 +1934,9 @@
       <c r="F12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1960,7 +1976,9 @@
       <c r="F13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -2000,7 +2018,9 @@
       <c r="F14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="1"/>
+      <c r="G14" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -2040,7 +2060,9 @@
       <c r="F15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="1"/>
+      <c r="G15" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -2080,7 +2102,9 @@
       <c r="F16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="1"/>
+      <c r="G16" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -2120,7 +2144,9 @@
       <c r="F17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="1"/>
+      <c r="G17" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -2160,7 +2186,9 @@
       <c r="F18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="1"/>
+      <c r="G18" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -2200,7 +2228,9 @@
       <c r="F19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G19" s="1"/>
+      <c r="G19" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -2240,7 +2270,9 @@
       <c r="F20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="1"/>
+      <c r="G20" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -2280,7 +2312,9 @@
       <c r="F21" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G21" s="1"/>
+      <c r="G21" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -2320,7 +2354,9 @@
       <c r="F22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G22" s="1"/>
+      <c r="G22" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -2360,7 +2396,9 @@
       <c r="F23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G23" s="1"/>
+      <c r="G23" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -2400,7 +2438,9 @@
       <c r="F24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G24" s="1"/>
+      <c r="G24" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -2440,7 +2480,9 @@
       <c r="F25" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G25" s="1"/>
+      <c r="G25" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -2480,7 +2522,9 @@
       <c r="F26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="1"/>
+      <c r="G26" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -2520,7 +2564,9 @@
       <c r="F27" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G27" s="1"/>
+      <c r="G27" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -2560,7 +2606,9 @@
       <c r="F28" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G28" s="1"/>
+      <c r="G28" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -2600,7 +2648,9 @@
       <c r="F29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G29" s="1"/>
+      <c r="G29" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -2640,7 +2690,9 @@
       <c r="F30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G30" s="1"/>
+      <c r="G30" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -2680,7 +2732,9 @@
       <c r="F31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="1"/>
+      <c r="G31" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -2720,7 +2774,9 @@
       <c r="F32" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G32" s="1"/>
+      <c r="G32" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -2760,7 +2816,9 @@
       <c r="F33" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G33" s="1"/>
+      <c r="G33" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -2800,7 +2858,9 @@
       <c r="F34" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G34" s="1"/>
+      <c r="G34" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -2840,7 +2900,9 @@
       <c r="F35" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G35" s="1"/>
+      <c r="G35" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
@@ -2880,7 +2942,9 @@
       <c r="F36" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G36" s="1"/>
+      <c r="G36" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
@@ -2920,7 +2984,9 @@
       <c r="F37" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G37" s="1"/>
+      <c r="G37" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
@@ -2960,7 +3026,9 @@
       <c r="F38" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G38" s="1"/>
+      <c r="G38" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
@@ -3000,7 +3068,9 @@
       <c r="F39" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G39" s="1"/>
+      <c r="G39" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
@@ -3040,7 +3110,9 @@
       <c r="F40" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G40" s="1"/>
+      <c r="G40" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
@@ -3080,7 +3152,9 @@
       <c r="F41" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G41" s="1"/>
+      <c r="G41" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
@@ -3120,7 +3194,9 @@
       <c r="F42" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G42" s="1"/>
+      <c r="G42" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -3160,7 +3236,9 @@
       <c r="F43" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G43" s="1"/>
+      <c r="G43" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
@@ -3200,7 +3278,9 @@
       <c r="F44" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G44" s="1"/>
+      <c r="G44" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>

</xml_diff>

<commit_message>
Buổi 11: nested router - layout
</commit_message>
<xml_diff>
--- a/diem_danh_giay_06_03_23_07_39_59.xlsx
+++ b/diem_danh_giay_06_03_23_07_39_59.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowHeight="16400"/>
+    <workbookView windowHeight="18800"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>dungntph20018@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
   <si>
     <t>PH20377</t>
@@ -132,9 +135,6 @@
   </si>
   <si>
     <t>truongvhph24614@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>A</t>
   </si>
   <si>
     <t>PH24621</t>
@@ -423,11 +423,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="dd\-mmm"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="dd\-mmm"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -485,6 +485,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -494,7 +517,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -509,23 +540,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -539,8 +568,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -563,52 +608,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -641,7 +641,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -653,13 +665,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -671,19 +695,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -695,7 +713,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -707,7 +725,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -719,13 +779,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -737,73 +803,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -847,6 +847,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -865,19 +883,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -899,169 +921,147 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1494,8 +1494,8 @@
   <sheetPr/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1643,7 +1643,9 @@
       <c r="G5" s="12">
         <v>45000</v>
       </c>
-      <c r="H5" s="1"/>
+      <c r="H5" s="12">
+        <v>45009</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -1686,7 +1688,9 @@
         <v>8</v>
       </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="I6" s="1">
+        <v>9</v>
+      </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -1728,7 +1732,9 @@
         <v>8</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="I7" s="1">
+        <v>9</v>
+      </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -1769,8 +1775,12 @@
       <c r="G8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="1">
+        <v>9</v>
+      </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -1794,13 +1804,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>8</v>
@@ -1812,7 +1822,9 @@
         <v>8</v>
       </c>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="I9" s="1">
+        <v>9</v>
+      </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -1836,13 +1848,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>8</v>
@@ -1854,7 +1866,9 @@
         <v>8</v>
       </c>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="I10" s="1">
+        <v>9</v>
+      </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -1878,13 +1892,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>8</v>
@@ -1896,7 +1910,9 @@
         <v>8</v>
       </c>
       <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="I11" s="1">
+        <v>9</v>
+      </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -1920,13 +1936,13 @@
         <v>7</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>8</v>
@@ -1938,7 +1954,9 @@
         <v>8</v>
       </c>
       <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="I12" s="1">
+        <v>9</v>
+      </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -1962,13 +1980,13 @@
         <v>8</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>8</v>
@@ -1980,7 +1998,9 @@
         <v>8</v>
       </c>
       <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="I13" s="1">
+        <v>4</v>
+      </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -2004,13 +2024,13 @@
         <v>9</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>8</v>
@@ -2022,7 +2042,9 @@
         <v>8</v>
       </c>
       <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+      <c r="I14" s="1">
+        <v>9</v>
+      </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -2046,13 +2068,13 @@
         <v>10</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>8</v>
@@ -2063,8 +2085,12 @@
       <c r="G15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="H15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="1">
+        <v>9</v>
+      </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -2088,16 +2114,16 @@
         <v>11</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>8</v>
@@ -2106,7 +2132,9 @@
         <v>8</v>
       </c>
       <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+      <c r="I16" s="1">
+        <v>9</v>
+      </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -2148,7 +2176,9 @@
         <v>8</v>
       </c>
       <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+      <c r="I17" s="1">
+        <v>9</v>
+      </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -2189,8 +2219,12 @@
       <c r="G18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="1">
+        <v>4</v>
+      </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -2232,7 +2266,9 @@
         <v>8</v>
       </c>
       <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
+      <c r="I19" s="1">
+        <v>9</v>
+      </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -2274,7 +2310,9 @@
         <v>8</v>
       </c>
       <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
+      <c r="I20" s="1">
+        <v>9</v>
+      </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -2307,16 +2345,20 @@
         <v>54</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0</v>
+      </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -2358,7 +2400,9 @@
         <v>8</v>
       </c>
       <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
+      <c r="I22" s="1">
+        <v>9</v>
+      </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -2391,7 +2435,7 @@
         <v>60</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>8</v>
@@ -2400,7 +2444,9 @@
         <v>8</v>
       </c>
       <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
+      <c r="I23" s="1">
+        <v>9</v>
+      </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -2442,7 +2488,9 @@
         <v>8</v>
       </c>
       <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
+      <c r="I24" s="1">
+        <v>4</v>
+      </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -2484,7 +2532,9 @@
         <v>8</v>
       </c>
       <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
+      <c r="I25" s="1">
+        <v>9</v>
+      </c>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -2526,7 +2576,9 @@
         <v>8</v>
       </c>
       <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
+      <c r="I26" s="1">
+        <v>9</v>
+      </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -2562,13 +2614,15 @@
         <v>8</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
+      <c r="I27" s="1">
+        <v>4</v>
+      </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -2604,13 +2658,15 @@
         <v>8</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
+      <c r="I28" s="1">
+        <v>4</v>
+      </c>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -2652,7 +2708,9 @@
         <v>8</v>
       </c>
       <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
+      <c r="I29" s="1">
+        <v>9</v>
+      </c>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
@@ -2685,7 +2743,7 @@
         <v>81</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>8</v>
@@ -2693,8 +2751,12 @@
       <c r="G30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
+      <c r="H30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I30" s="1">
+        <v>9</v>
+      </c>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
@@ -2727,7 +2789,7 @@
         <v>84</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>8</v>
@@ -2736,7 +2798,9 @@
         <v>8</v>
       </c>
       <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
+      <c r="I31" s="1">
+        <v>9</v>
+      </c>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -2778,7 +2842,9 @@
         <v>8</v>
       </c>
       <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
+      <c r="I32" s="1">
+        <v>9</v>
+      </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
@@ -2819,8 +2885,12 @@
       <c r="G33" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
+      <c r="H33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I33" s="1">
+        <v>9</v>
+      </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
@@ -2862,7 +2932,9 @@
         <v>8</v>
       </c>
       <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
+      <c r="I34" s="1">
+        <v>9</v>
+      </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
@@ -2904,7 +2976,9 @@
         <v>8</v>
       </c>
       <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
+      <c r="I35" s="1">
+        <v>9</v>
+      </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
@@ -2946,7 +3020,9 @@
         <v>8</v>
       </c>
       <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
+      <c r="I36" s="1">
+        <v>9</v>
+      </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
@@ -2979,7 +3055,7 @@
         <v>102</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>8</v>
@@ -2988,7 +3064,9 @@
         <v>8</v>
       </c>
       <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
+      <c r="I37" s="1">
+        <v>9</v>
+      </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
@@ -3024,13 +3102,15 @@
         <v>8</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
+      <c r="I38" s="1">
+        <v>9</v>
+      </c>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
@@ -3072,7 +3152,9 @@
         <v>8</v>
       </c>
       <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
+      <c r="I39" s="1">
+        <v>9</v>
+      </c>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
@@ -3114,7 +3196,9 @@
         <v>8</v>
       </c>
       <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
+      <c r="I40" s="1">
+        <v>9</v>
+      </c>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
@@ -3147,16 +3231,20 @@
         <v>114</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="F41" s="13" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I41" s="1">
+        <v>0</v>
+      </c>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
@@ -3198,7 +3286,9 @@
         <v>8</v>
       </c>
       <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
+      <c r="I42" s="1">
+        <v>9</v>
+      </c>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
@@ -3240,7 +3330,9 @@
         <v>8</v>
       </c>
       <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
+      <c r="I43" s="1">
+        <v>9</v>
+      </c>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
@@ -3273,7 +3365,7 @@
         <v>123</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>8</v>
@@ -3282,7 +3374,9 @@
         <v>8</v>
       </c>
       <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
+      <c r="I44" s="1">
+        <v>9</v>
+      </c>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>

</xml_diff>

<commit_message>
Buổi 12: ant design - add product
</commit_message>
<xml_diff>
--- a/diem_danh_giay_06_03_23_07_39_59.xlsx
+++ b/diem_danh_giay_06_03_23_07_39_59.xlsx
@@ -423,11 +423,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="dd\-mmm"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="dd\-mmm"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -478,10 +478,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -493,33 +493,10 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -546,15 +523,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -563,6 +549,21 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -577,29 +578,19 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -607,8 +598,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -623,7 +623,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -635,157 +683,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -803,7 +713,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -828,21 +828,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -880,15 +865,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -919,6 +895,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -929,148 +920,157 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1494,8 +1494,8 @@
   <sheetPr/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1504,7 +1504,8 @@
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="29.421875" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="5" max="8" width="3.2890625" customWidth="1"/>
+    <col min="9" max="9" width="4.0390625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -1647,7 +1648,9 @@
         <v>45009</v>
       </c>
       <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="J5" s="12">
+        <v>45016</v>
+      </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -1781,7 +1784,9 @@
       <c r="I8" s="1">
         <v>9</v>
       </c>
-      <c r="J8" s="1"/>
+      <c r="J8" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -2359,7 +2364,9 @@
       <c r="I21" s="1">
         <v>0</v>
       </c>
-      <c r="J21" s="1"/>
+      <c r="J21" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -2447,7 +2454,9 @@
       <c r="I23" s="1">
         <v>9</v>
       </c>
-      <c r="J23" s="1"/>
+      <c r="J23" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -2579,7 +2588,9 @@
       <c r="I26" s="1">
         <v>9</v>
       </c>
-      <c r="J26" s="1"/>
+      <c r="J26" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -2667,7 +2678,9 @@
       <c r="I28" s="1">
         <v>4</v>
       </c>
-      <c r="J28" s="1"/>
+      <c r="J28" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -2845,7 +2858,9 @@
       <c r="I32" s="1">
         <v>9</v>
       </c>
-      <c r="J32" s="1"/>
+      <c r="J32" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -2979,7 +2994,9 @@
       <c r="I35" s="1">
         <v>9</v>
       </c>
-      <c r="J35" s="1"/>
+      <c r="J35" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -3245,7 +3262,9 @@
       <c r="I41" s="1">
         <v>0</v>
       </c>
-      <c r="J41" s="1"/>
+      <c r="J41" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
@@ -3289,7 +3308,9 @@
       <c r="I42" s="1">
         <v>9</v>
       </c>
-      <c r="J42" s="1"/>
+      <c r="J42" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>

</xml_diff>